<commit_message>
Update Sage scrape results
</commit_message>
<xml_diff>
--- a/sage_scrape_results.xlsx
+++ b/sage_scrape_results.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,992 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Search Term</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Authors</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>DOI</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Access Type</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estonia 2007</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Bronze Soldier</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Georgia 2008</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Russo-Georgian War</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Stuxnet</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Olympic Games</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Shamoon</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Saudi Aramco</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Ras Gas</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Sony</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>The Interview</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>DNC</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Guccifer 2.0</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Democratic National Committee</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Ukrainian Power Grid</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>BlackEnergy 3</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Sandowrm</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Considering the cost of cyber warfare: advancing cyber warfare analytics to better assess tradeoffs in system destruction warfare</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Considering the cost of cyber warfare: advancing cyber warfare analytics to better assess tradeoffs in system destruction warfare</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Technical note: exploiting problem definition study for cyber security simulations</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Technical note: exploiting problem definition study for cyber security simulations</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Warring from the virtual to the real: Assessing the public’s threshold for war over cyber security</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Responding to Uncertainty: The Importance of Covertness in Support for Retaliation to Cyber and Kinetic Attacks</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Cyber and contentious politics: Evidence from the US radical environmental movement</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Accountability and cyber conflict: examining institutional constraints on the use of cyber proxies</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Accountability and cyber conflict: examining institutional constraints on the use of cyber proxies</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kinetic Cyber</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Invisible Digital Front: Can Cyber Attacks Shape Battlefield Events?</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Restricted</t>
+        </is>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>